<commit_message>
Uploaded images of test results
</commit_message>
<xml_diff>
--- a/Risultati/Risultati Bot.xlsx
+++ b/Risultati/Risultati Bot.xlsx
@@ -486,8 +486,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="295798528"/>
-        <c:axId val="295798136"/>
+        <c:axId val="268540384"/>
+        <c:axId val="268540000"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -693,11 +693,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="295797744"/>
-        <c:axId val="295800096"/>
+        <c:axId val="267265472"/>
+        <c:axId val="267268216"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="295798136"/>
+        <c:axId val="268540000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,12 +747,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295798528"/>
+        <c:crossAx val="268540384"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="295798528"/>
+        <c:axId val="268540384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -794,7 +794,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295798136"/>
+        <c:crossAx val="268540000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -802,7 +802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="295800096"/>
+        <c:axId val="267268216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,12 +838,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295797744"/>
+        <c:crossAx val="267265472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="295797744"/>
+        <c:axId val="267265472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +852,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="295800096"/>
+        <c:crossAx val="267268216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1481,8 +1481,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="298278296"/>
-        <c:axId val="298276336"/>
+        <c:axId val="269392368"/>
+        <c:axId val="269391976"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1726,11 +1726,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="297110752"/>
-        <c:axId val="298278688"/>
+        <c:axId val="269398640"/>
+        <c:axId val="269397072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297110752"/>
+        <c:axId val="269398640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1772,7 +1772,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298278688"/>
+        <c:crossAx val="269397072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1780,7 +1780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298278688"/>
+        <c:axId val="269397072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,12 +1830,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297110752"/>
+        <c:crossAx val="269398640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="298276336"/>
+        <c:axId val="269391976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,12 +1871,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298278296"/>
+        <c:crossAx val="269392368"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="298278296"/>
+        <c:axId val="269392368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1886,7 +1886,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298276336"/>
+        <c:crossAx val="269391976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2507,8 +2507,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="298276728"/>
-        <c:axId val="298277512"/>
+        <c:axId val="268337480"/>
+        <c:axId val="268337088"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2752,11 +2752,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="298283000"/>
-        <c:axId val="298277120"/>
+        <c:axId val="268335520"/>
+        <c:axId val="268336696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="298283000"/>
+        <c:axId val="268335520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +2798,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298277120"/>
+        <c:crossAx val="268336696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2806,7 +2806,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="298277120"/>
+        <c:axId val="268336696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2856,12 +2856,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298283000"/>
+        <c:crossAx val="268335520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="298277512"/>
+        <c:axId val="268337088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2897,12 +2897,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298276728"/>
+        <c:crossAx val="268337480"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="298276728"/>
+        <c:axId val="268337480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2912,7 +2912,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="298277512"/>
+        <c:crossAx val="268337088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3292,8 +3292,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="350302984"/>
-        <c:axId val="350309256"/>
+        <c:axId val="267453728"/>
+        <c:axId val="267453336"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3499,11 +3499,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350303768"/>
-        <c:axId val="350302592"/>
+        <c:axId val="267456080"/>
+        <c:axId val="267454120"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="350309256"/>
+        <c:axId val="267453336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3553,12 +3553,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350302984"/>
+        <c:crossAx val="267453728"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350302984"/>
+        <c:axId val="267453728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3600,7 +3600,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350309256"/>
+        <c:crossAx val="267453336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3608,7 +3608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350302592"/>
+        <c:axId val="267454120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3644,12 +3644,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350303768"/>
+        <c:crossAx val="267456080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350303768"/>
+        <c:axId val="267456080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3658,7 +3658,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350302592"/>
+        <c:crossAx val="267454120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4075,8 +4075,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="350306512"/>
-        <c:axId val="350306120"/>
+        <c:axId val="267455296"/>
+        <c:axId val="267452552"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4320,11 +4320,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350308864"/>
-        <c:axId val="350304944"/>
+        <c:axId val="267454904"/>
+        <c:axId val="267454512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350308864"/>
+        <c:axId val="267454904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4366,7 +4366,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350304944"/>
+        <c:crossAx val="267454512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4374,7 +4374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350304944"/>
+        <c:axId val="267454512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4424,12 +4424,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350308864"/>
+        <c:crossAx val="267454904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350306120"/>
+        <c:axId val="267452552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4465,12 +4465,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350306512"/>
+        <c:crossAx val="267455296"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350306512"/>
+        <c:axId val="267455296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4480,7 +4480,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350306120"/>
+        <c:crossAx val="267452552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4897,8 +4897,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="350368592"/>
-        <c:axId val="350362320"/>
+        <c:axId val="267458432"/>
+        <c:axId val="267457256"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5142,11 +5142,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350363104"/>
-        <c:axId val="350361928"/>
+        <c:axId val="267459216"/>
+        <c:axId val="267456472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350363104"/>
+        <c:axId val="267459216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5188,7 +5188,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350361928"/>
+        <c:crossAx val="267456472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5196,7 +5196,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350361928"/>
+        <c:axId val="267456472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5246,12 +5246,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350363104"/>
+        <c:crossAx val="267459216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350362320"/>
+        <c:axId val="267457256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5287,12 +5287,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350368592"/>
+        <c:crossAx val="267458432"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350368592"/>
+        <c:axId val="267458432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5302,7 +5302,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350362320"/>
+        <c:crossAx val="267457256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5770,8 +5770,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="350359576"/>
-        <c:axId val="350368984"/>
+        <c:axId val="309143080"/>
+        <c:axId val="267452160"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6015,11 +6015,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350362712"/>
-        <c:axId val="350367416"/>
+        <c:axId val="267458824"/>
+        <c:axId val="267459608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350362712"/>
+        <c:axId val="267458824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6061,7 +6061,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350367416"/>
+        <c:crossAx val="267459608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6069,7 +6069,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350367416"/>
+        <c:axId val="267459608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6119,12 +6119,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350362712"/>
+        <c:crossAx val="267458824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350368984"/>
+        <c:axId val="267452160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6160,12 +6160,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350359576"/>
+        <c:crossAx val="309143080"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350359576"/>
+        <c:axId val="309143080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6175,7 +6175,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350368984"/>
+        <c:crossAx val="267452160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6694,8 +6694,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="350366632"/>
-        <c:axId val="350366240"/>
+        <c:axId val="309142296"/>
+        <c:axId val="309139160"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6939,11 +6939,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350364672"/>
-        <c:axId val="350365848"/>
+        <c:axId val="309143864"/>
+        <c:axId val="309141904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350364672"/>
+        <c:axId val="309143864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6985,7 +6985,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350365848"/>
+        <c:crossAx val="309141904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6993,7 +6993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350365848"/>
+        <c:axId val="309141904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7043,12 +7043,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350364672"/>
+        <c:crossAx val="309143864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350366240"/>
+        <c:axId val="309139160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7084,12 +7084,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350366632"/>
+        <c:crossAx val="309142296"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350366632"/>
+        <c:axId val="309142296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7099,7 +7099,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350366240"/>
+        <c:crossAx val="309139160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7677,8 +7677,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="350367024"/>
-        <c:axId val="350359968"/>
+        <c:axId val="309141512"/>
+        <c:axId val="309144256"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7922,11 +7922,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350364280"/>
-        <c:axId val="350361144"/>
+        <c:axId val="309142688"/>
+        <c:axId val="309141120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350364280"/>
+        <c:axId val="309142688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7968,7 +7968,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350361144"/>
+        <c:crossAx val="309141120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7976,7 +7976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350361144"/>
+        <c:axId val="309141120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8026,12 +8026,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350364280"/>
+        <c:crossAx val="309142688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350359968"/>
+        <c:axId val="309144256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8067,12 +8067,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350367024"/>
+        <c:crossAx val="309141512"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350367024"/>
+        <c:axId val="309141512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8082,7 +8082,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350359968"/>
+        <c:crossAx val="309144256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8507,11 +8507,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="350365064"/>
-        <c:axId val="350367808"/>
+        <c:axId val="309144648"/>
+        <c:axId val="309145040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350365064"/>
+        <c:axId val="309144648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8553,7 +8553,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350367808"/>
+        <c:crossAx val="309145040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8561,7 +8561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350367808"/>
+        <c:axId val="309145040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8611,7 +8611,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350365064"/>
+        <c:crossAx val="309144648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9229,8 +9229,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="350370552"/>
-        <c:axId val="350369768"/>
+        <c:axId val="309140336"/>
+        <c:axId val="309139552"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9474,11 +9474,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350370160"/>
-        <c:axId val="350369376"/>
+        <c:axId val="309146216"/>
+        <c:axId val="309146608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350370160"/>
+        <c:axId val="309146216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9520,7 +9520,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350369376"/>
+        <c:crossAx val="309146608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9528,7 +9528,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350369376"/>
+        <c:axId val="309146608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9578,12 +9578,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350370160"/>
+        <c:crossAx val="309146216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350369768"/>
+        <c:axId val="309139552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9619,12 +9619,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350370552"/>
+        <c:crossAx val="309140336"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350370552"/>
+        <c:axId val="309140336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9634,7 +9634,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350369768"/>
+        <c:crossAx val="309139552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10051,8 +10051,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="297111144"/>
-        <c:axId val="297113888"/>
+        <c:axId val="267266256"/>
+        <c:axId val="267265864"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -10296,11 +10296,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="297109184"/>
-        <c:axId val="297113496"/>
+        <c:axId val="267267040"/>
+        <c:axId val="267265080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297109184"/>
+        <c:axId val="267267040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10342,7 +10342,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297113496"/>
+        <c:crossAx val="267265080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10350,7 +10350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297113496"/>
+        <c:axId val="267265080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10400,12 +10400,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297109184"/>
+        <c:crossAx val="267267040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297113888"/>
+        <c:axId val="267265864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10441,12 +10441,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297111144"/>
+        <c:crossAx val="267266256"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="297111144"/>
+        <c:axId val="267266256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10456,7 +10456,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297113888"/>
+        <c:crossAx val="267265864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11077,8 +11077,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="350359184"/>
-        <c:axId val="350371336"/>
+        <c:axId val="309574696"/>
+        <c:axId val="309578224"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -11322,11 +11322,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350360360"/>
-        <c:axId val="350365456"/>
+        <c:axId val="309582144"/>
+        <c:axId val="309579400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350360360"/>
+        <c:axId val="309582144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11368,7 +11368,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350365456"/>
+        <c:crossAx val="309579400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11376,7 +11376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350365456"/>
+        <c:axId val="309579400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11426,12 +11426,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350360360"/>
+        <c:crossAx val="309582144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350371336"/>
+        <c:axId val="309578224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11467,12 +11467,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350359184"/>
+        <c:crossAx val="309574696"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350359184"/>
+        <c:axId val="309574696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11482,7 +11482,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350371336"/>
+        <c:crossAx val="309578224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12111,8 +12111,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="350373296"/>
-        <c:axId val="350372120"/>
+        <c:axId val="309581360"/>
+        <c:axId val="309577440"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12356,11 +12356,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350371728"/>
-        <c:axId val="350373688"/>
+        <c:axId val="309575088"/>
+        <c:axId val="309577832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350371728"/>
+        <c:axId val="309575088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12402,7 +12402,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350373688"/>
+        <c:crossAx val="309577832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12410,7 +12410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350373688"/>
+        <c:axId val="309577832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12460,12 +12460,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350371728"/>
+        <c:crossAx val="309575088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350372120"/>
+        <c:axId val="309577440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12501,12 +12501,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350373296"/>
+        <c:crossAx val="309581360"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="350373296"/>
+        <c:axId val="309581360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12516,7 +12516,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350372120"/>
+        <c:crossAx val="309577440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13137,8 +13137,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="399344144"/>
-        <c:axId val="350372904"/>
+        <c:axId val="309575872"/>
+        <c:axId val="309575480"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -13382,11 +13382,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="350372512"/>
-        <c:axId val="350374080"/>
+        <c:axId val="309581752"/>
+        <c:axId val="309579008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="350372512"/>
+        <c:axId val="309581752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13428,7 +13428,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350374080"/>
+        <c:crossAx val="309579008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13436,7 +13436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="350374080"/>
+        <c:axId val="309579008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13486,12 +13486,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="350372512"/>
+        <c:crossAx val="309581752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="350372904"/>
+        <c:axId val="309575480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13527,12 +13527,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399344144"/>
+        <c:crossAx val="309575872"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="399344144"/>
+        <c:axId val="309575872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13542,7 +13542,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="350372904"/>
+        <c:crossAx val="309575480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14034,8 +14034,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="412137120"/>
-        <c:axId val="412128104"/>
+        <c:axId val="309576656"/>
+        <c:axId val="309576264"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14434,11 +14434,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="412143000"/>
-        <c:axId val="412128888"/>
+        <c:axId val="309580184"/>
+        <c:axId val="309577048"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="412128104"/>
+        <c:axId val="309576264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14488,12 +14488,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412137120"/>
+        <c:crossAx val="309576656"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="412137120"/>
+        <c:axId val="309576656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14535,7 +14535,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412128104"/>
+        <c:crossAx val="309576264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14543,7 +14543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412128888"/>
+        <c:axId val="309577048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14579,12 +14579,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412143000"/>
+        <c:crossAx val="309580184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="412143000"/>
+        <c:axId val="309580184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14593,7 +14593,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412128888"/>
+        <c:crossAx val="309577048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14932,8 +14932,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="401525632"/>
-        <c:axId val="553147840"/>
+        <c:axId val="309896408"/>
+        <c:axId val="309899544"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -15110,11 +15110,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="403027208"/>
-        <c:axId val="403020152"/>
+        <c:axId val="309900328"/>
+        <c:axId val="309900720"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="403020152"/>
+        <c:axId val="309900720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15164,12 +15164,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="403027208"/>
+        <c:crossAx val="309900328"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="403027208"/>
+        <c:axId val="309900328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15211,7 +15211,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="403020152"/>
+        <c:crossAx val="309900720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15219,7 +15219,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="553147840"/>
+        <c:axId val="309899544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15255,11 +15255,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="401525632"/>
+        <c:crossAx val="309896408"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="401525632"/>
+        <c:axId val="309896408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15269,7 +15270,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="553147840"/>
+        <c:crossAx val="309899544"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -15654,8 +15656,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="459639616"/>
-        <c:axId val="459639224"/>
+        <c:axId val="309898760"/>
+        <c:axId val="309894448"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -15938,11 +15940,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="459638048"/>
-        <c:axId val="459638832"/>
+        <c:axId val="309899152"/>
+        <c:axId val="309899936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="459638048"/>
+        <c:axId val="309899152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15984,7 +15986,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459638832"/>
+        <c:crossAx val="309899936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15992,7 +15994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="459638832"/>
+        <c:axId val="309899936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16042,12 +16044,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459638048"/>
+        <c:crossAx val="309899152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="459639224"/>
+        <c:axId val="309894448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16083,12 +16085,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459639616"/>
+        <c:crossAx val="309898760"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="459639616"/>
+        <c:axId val="309898760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16098,7 +16100,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="459639224"/>
+        <c:crossAx val="309894448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16645,8 +16647,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="459617272"/>
-        <c:axId val="459618840"/>
+        <c:axId val="309895232"/>
+        <c:axId val="309894840"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -16929,11 +16931,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="459620408"/>
-        <c:axId val="459614528"/>
+        <c:axId val="309901504"/>
+        <c:axId val="309897192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="459620408"/>
+        <c:axId val="309901504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16975,7 +16977,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459614528"/>
+        <c:crossAx val="309897192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16983,7 +16985,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="459614528"/>
+        <c:axId val="309897192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17033,12 +17035,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459620408"/>
+        <c:crossAx val="309901504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="459618840"/>
+        <c:axId val="309894840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17074,12 +17076,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459617272"/>
+        <c:crossAx val="309895232"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="459617272"/>
+        <c:axId val="309895232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17089,7 +17091,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="459618840"/>
+        <c:crossAx val="309894840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17679,8 +17681,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="412139080"/>
-        <c:axId val="412127712"/>
+        <c:axId val="309896800"/>
+        <c:axId val="309896016"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -17963,11 +17965,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="412131240"/>
-        <c:axId val="412132808"/>
+        <c:axId val="309898368"/>
+        <c:axId val="309895624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412131240"/>
+        <c:axId val="309898368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18009,7 +18011,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412132808"/>
+        <c:crossAx val="309895624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18017,7 +18019,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412132808"/>
+        <c:axId val="309895624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18067,12 +18069,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412131240"/>
+        <c:crossAx val="309898368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412127712"/>
+        <c:axId val="309896016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18108,12 +18110,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412139080"/>
+        <c:crossAx val="309896800"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="412139080"/>
+        <c:axId val="309896800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18123,7 +18125,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412127712"/>
+        <c:crossAx val="309896016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18462,8 +18464,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="507605008"/>
-        <c:axId val="507604616"/>
+        <c:axId val="310802936"/>
+        <c:axId val="310804504"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -18657,11 +18659,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="412145352"/>
-        <c:axId val="412141432"/>
+        <c:axId val="310803328"/>
+        <c:axId val="310798232"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="412141432"/>
+        <c:axId val="310798232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18711,12 +18713,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412145352"/>
+        <c:crossAx val="310803328"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="412145352"/>
+        <c:axId val="310803328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18758,7 +18760,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412141432"/>
+        <c:crossAx val="310798232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18766,7 +18768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="507604616"/>
+        <c:axId val="310804504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18802,11 +18804,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507605008"/>
+        <c:crossAx val="310802936"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="507605008"/>
+        <c:axId val="310802936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18816,7 +18819,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="507604616"/>
+        <c:crossAx val="310804504"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -19201,8 +19205,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="412120656"/>
-        <c:axId val="412123400"/>
+        <c:axId val="310800976"/>
+        <c:axId val="310800584"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -19485,11 +19489,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="412119872"/>
-        <c:axId val="412124968"/>
+        <c:axId val="310801760"/>
+        <c:axId val="310799800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412119872"/>
+        <c:axId val="310801760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19531,7 +19535,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412124968"/>
+        <c:crossAx val="310799800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19539,7 +19543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412124968"/>
+        <c:axId val="310799800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19589,12 +19593,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412119872"/>
+        <c:crossAx val="310801760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412123400"/>
+        <c:axId val="310800584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19630,12 +19634,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412120656"/>
+        <c:crossAx val="310800976"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="412120656"/>
+        <c:axId val="310800976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19645,7 +19649,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412123400"/>
+        <c:crossAx val="310800584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20062,8 +20066,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="297106832"/>
-        <c:axId val="297109968"/>
+        <c:axId val="268330424"/>
+        <c:axId val="268332776"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -20307,11 +20311,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="297109576"/>
-        <c:axId val="297108792"/>
+        <c:axId val="267267432"/>
+        <c:axId val="267267824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297109576"/>
+        <c:axId val="267267432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20353,7 +20357,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297108792"/>
+        <c:crossAx val="267267824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20361,7 +20365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297108792"/>
+        <c:axId val="267267824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20411,12 +20415,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297109576"/>
+        <c:crossAx val="267267432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297109968"/>
+        <c:axId val="268332776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20452,12 +20456,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297106832"/>
+        <c:crossAx val="268330424"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="297106832"/>
+        <c:axId val="268330424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20467,7 +20471,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297109968"/>
+        <c:crossAx val="268332776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20957,6 +20961,12 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'GSP (random)'!#REF!</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'FPA (random)'!$C$22:$C$31</c:f>
@@ -20996,23 +21006,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredCategoryTitle>
-                <c15:cat>
-                  <c:multiLvlStrRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'GSP (random)'!#REF!</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                  </c:multiLvlStrRef>
-                </c15:cat>
-              </c15:filteredCategoryTitle>
-            </c:ext>
-          </c:extLst>
+          <c:extLst/>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="ctr"/>
@@ -21024,8 +21018,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="412121832"/>
-        <c:axId val="412118304"/>
+        <c:axId val="310802544"/>
+        <c:axId val="310805288"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -21057,6 +21051,44 @@
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FPA (random)'!$B$22:$B$31</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>best_response</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>best_response_competitive</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>best_response_altruistic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>competitor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>budget_saving</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>random</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>competitor_budget</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>preferential_competitor</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>best_competitor_budget</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>best_preferential_competitor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>('FPA (random)'!$D$32,'FPA (random)'!$D$32,'FPA (random)'!$D$32,'FPA (random)'!$D$32,'FPA (random)'!$D$32,'FPA (random)'!$D$32,'FPA (random)'!$D$32,'FPA (random)'!$D$32,'FPA (random)'!$D$32,'FPA (random)'!$D$32)</c:f>
@@ -21179,6 +21211,44 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FPA (random)'!$B$22:$B$31</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>best_response</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>best_response_competitive</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>best_response_altruistic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>competitor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>budget_saving</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>random</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>competitor_budget</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>preferential_competitor</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>best_competitor_budget</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>best_preferential_competitor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'FPA (random)'!$D$22:$D$31</c:f>
@@ -21219,23 +21289,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredCategoryTitle>
-                <c15:cat>
-                  <c:multiLvlStrRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'GSP (random)'!#REF!</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                  </c:multiLvlStrRef>
-                </c15:cat>
-              </c15:filteredCategoryTitle>
-            </c:ext>
-          </c:extLst>
+          <c:extLst/>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="ctr"/>
@@ -21248,11 +21302,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="412125360"/>
-        <c:axId val="412114384"/>
+        <c:axId val="310802152"/>
+        <c:axId val="310804896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412125360"/>
+        <c:axId val="310802152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21294,7 +21348,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412114384"/>
+        <c:crossAx val="310804896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21302,7 +21356,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412114384"/>
+        <c:axId val="310804896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21352,12 +21406,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412125360"/>
+        <c:crossAx val="310802152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412118304"/>
+        <c:axId val="310805288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21393,12 +21447,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412121832"/>
+        <c:crossAx val="310802544"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="412121832"/>
+        <c:axId val="310802544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21408,7 +21462,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412118304"/>
+        <c:crossAx val="310805288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21941,6 +21995,12 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'GSP (random)'!#REF!</c:f>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'FPA (random)'!$C$42:$C$51</c:f>
@@ -21980,23 +22040,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredCategoryTitle>
-                <c15:cat>
-                  <c:multiLvlStrRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'GSP (random)'!#REF!</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                  </c:multiLvlStrRef>
-                </c15:cat>
-              </c15:filteredCategoryTitle>
-            </c:ext>
-          </c:extLst>
+          <c:extLst/>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="ctr"/>
@@ -22008,8 +22052,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="412115168"/>
-        <c:axId val="412123008"/>
+        <c:axId val="310800192"/>
+        <c:axId val="310799408"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -22041,6 +22085,44 @@
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FPA (random)'!$B$42:$B$51</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>best_response</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>best_response_competitive</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>best_response_altruistic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>competitor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>budget_saving</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>random</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>competitor_budget</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>preferential_competitor</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>best_competitor_budget</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>best_preferential_competitor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>('FPA (random)'!$D$52,'FPA (random)'!$D$52,'FPA (random)'!$D$52,'FPA (random)'!$D$52,'FPA (random)'!$D$52,'FPA (random)'!$D$52,'FPA (random)'!$D$52,'FPA (random)'!$D$52,'FPA (random)'!$D$52,'FPA (random)'!$D$52)</c:f>
@@ -22163,6 +22245,44 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FPA (random)'!$B$42:$B$51</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>best_response</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>best_response_competitive</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>best_response_altruistic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>competitor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>budget_saving</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>random</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>competitor_budget</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>preferential_competitor</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>best_competitor_budget</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>best_preferential_competitor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'FPA (random)'!$D$42:$D$51</c:f>
@@ -22203,23 +22323,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredCategoryTitle>
-                <c15:cat>
-                  <c:multiLvlStrRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'GSP (random)'!#REF!</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                  </c:multiLvlStrRef>
-                </c15:cat>
-              </c15:filteredCategoryTitle>
-            </c:ext>
-          </c:extLst>
+          <c:extLst/>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="ctr"/>
@@ -22232,11 +22336,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="412124184"/>
-        <c:axId val="412114776"/>
+        <c:axId val="310798624"/>
+        <c:axId val="310799016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412124184"/>
+        <c:axId val="310798624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22278,7 +22382,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412114776"/>
+        <c:crossAx val="310799016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22286,7 +22390,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412114776"/>
+        <c:axId val="310799016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22336,12 +22440,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412124184"/>
+        <c:crossAx val="310798624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412123008"/>
+        <c:axId val="310799408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22377,12 +22481,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412115168"/>
+        <c:crossAx val="310800192"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="412115168"/>
+        <c:axId val="310800192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22392,7 +22496,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="412123008"/>
+        <c:crossAx val="310799408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22860,8 +22964,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="297113104"/>
-        <c:axId val="297108400"/>
+        <c:axId val="268333560"/>
+        <c:axId val="268335912"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -23105,11 +23209,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="297107616"/>
-        <c:axId val="297108008"/>
+        <c:axId val="268333168"/>
+        <c:axId val="268336304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297107616"/>
+        <c:axId val="268333168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23151,7 +23255,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297108008"/>
+        <c:crossAx val="268336304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23159,7 +23263,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297108008"/>
+        <c:axId val="268336304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23209,12 +23313,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297107616"/>
+        <c:crossAx val="268333168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297108400"/>
+        <c:axId val="268335912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23250,12 +23354,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297113104"/>
+        <c:crossAx val="268333560"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="297113104"/>
+        <c:axId val="268333560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23265,7 +23369,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297108400"/>
+        <c:crossAx val="268335912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23784,8 +23888,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="297817800"/>
-        <c:axId val="297112712"/>
+        <c:axId val="268335128"/>
+        <c:axId val="268334736"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -24029,11 +24133,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="297111928"/>
-        <c:axId val="297112320"/>
+        <c:axId val="268332384"/>
+        <c:axId val="268330816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297111928"/>
+        <c:axId val="268332384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24075,7 +24179,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297112320"/>
+        <c:crossAx val="268330816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24083,7 +24187,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297112320"/>
+        <c:axId val="268330816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24133,12 +24237,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297111928"/>
+        <c:crossAx val="268332384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297112712"/>
+        <c:axId val="268334736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24174,12 +24278,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297817800"/>
+        <c:crossAx val="268335128"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="297817800"/>
+        <c:axId val="268335128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24189,7 +24293,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297112712"/>
+        <c:crossAx val="268334736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24767,8 +24871,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="297814664"/>
-        <c:axId val="297811528"/>
+        <c:axId val="269395896"/>
+        <c:axId val="268331992"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -25012,11 +25116,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="297814272"/>
-        <c:axId val="297812704"/>
+        <c:axId val="268331600"/>
+        <c:axId val="268330032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297814272"/>
+        <c:axId val="268331600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25058,7 +25162,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297812704"/>
+        <c:crossAx val="268330032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25066,7 +25170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297812704"/>
+        <c:axId val="268330032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25116,12 +25220,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297814272"/>
+        <c:crossAx val="268331600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297811528"/>
+        <c:axId val="268331992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25157,12 +25261,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297814664"/>
+        <c:crossAx val="269395896"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="297814664"/>
+        <c:axId val="269395896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25172,7 +25276,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297811528"/>
+        <c:crossAx val="268331992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25597,11 +25701,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297813096"/>
-        <c:axId val="297815840"/>
+        <c:axId val="269394720"/>
+        <c:axId val="269396288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297813096"/>
+        <c:axId val="269394720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25643,7 +25747,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297815840"/>
+        <c:crossAx val="269396288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25651,7 +25755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297815840"/>
+        <c:axId val="269396288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25701,7 +25805,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297813096"/>
+        <c:crossAx val="269394720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26319,8 +26423,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="297816232"/>
-        <c:axId val="297813488"/>
+        <c:axId val="269397856"/>
+        <c:axId val="269395504"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -26564,11 +26668,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="297810352"/>
-        <c:axId val="297815056"/>
+        <c:axId val="269393936"/>
+        <c:axId val="269395112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297810352"/>
+        <c:axId val="269393936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26610,7 +26714,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297815056"/>
+        <c:crossAx val="269395112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26618,7 +26722,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297815056"/>
+        <c:axId val="269395112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26668,12 +26772,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297810352"/>
+        <c:crossAx val="269393936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297813488"/>
+        <c:axId val="269395504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26709,12 +26813,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297816232"/>
+        <c:crossAx val="269397856"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="297816232"/>
+        <c:axId val="269397856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26724,7 +26828,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297813488"/>
+        <c:crossAx val="269395504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27345,8 +27449,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="297817408"/>
-        <c:axId val="297817016"/>
+        <c:axId val="269394328"/>
+        <c:axId val="269398248"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -27590,11 +27694,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="297816624"/>
-        <c:axId val="297811136"/>
+        <c:axId val="269393544"/>
+        <c:axId val="269397464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297816624"/>
+        <c:axId val="269393544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27636,7 +27740,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297811136"/>
+        <c:crossAx val="269397464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27644,7 +27748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297811136"/>
+        <c:axId val="269397464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27694,12 +27798,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297816624"/>
+        <c:crossAx val="269393544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297817016"/>
+        <c:axId val="269398248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27735,12 +27839,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297817408"/>
+        <c:crossAx val="269394328"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="297817408"/>
+        <c:axId val="269394328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27750,7 +27854,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297817016"/>
+        <c:crossAx val="269398248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -45377,15 +45481,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>47622</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>36737</xdr:rowOff>
+      <xdr:colOff>61230</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>376915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>27215</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:colOff>40823</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>353785</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -46289,7 +46393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C172" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
@@ -47929,8 +48033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="H2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H189" sqref="H189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
@@ -49539,7 +49643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="T6:W26"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
@@ -49633,7 +49737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B54" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -50173,8 +50277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>

</xml_diff>